<commit_message>
Rename Grammar Optimization to Grammar Transformation
</commit_message>
<xml_diff>
--- a/2_Supplemental_Material/Section_7_Evaluation/Subsection_7.1_Grammar_Adaptation/Metrics_SML.xlsx
+++ b/2_Supplemental_Material/Section_7_Evaluation/Subsection_7.1_Grammar_Adaptation/Metrics_SML.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.Git Repository\GrammarTransformer_data\2_Supplemental_Material\Section_7_Evaluation\Subsection_7.1_Grammar_Adaptation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C80D35-70DB-4A76-8CEF-66516134BAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -17,9 +26,6 @@
   </si>
   <si>
     <t>Generated Xtext Grammar</t>
-  </si>
-  <si>
-    <t>Optimized Grammar</t>
   </si>
   <si>
     <t>imitated</t>
@@ -862,30 +868,34 @@
          conditionExpression=ConditionExpression
     ']';</t>
   </si>
+  <si>
+    <t>Transformed Grammar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -896,7 +906,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -906,56 +916,56 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1145,766 +1155,772 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="70.63"/>
-    <col customWidth="1" min="2" max="2" width="81.38"/>
-    <col customWidth="1" min="3" max="3" width="59.5"/>
-    <col customWidth="1" min="6" max="6" width="40.63"/>
+    <col min="1" max="1" width="70.6328125" customWidth="1"/>
+    <col min="2" max="2" width="81.36328125" customWidth="1"/>
+    <col min="3" max="3" width="59.453125" customWidth="1"/>
+    <col min="6" max="6" width="40.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="287.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="100" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="100" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="125" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="100" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="8" t="s">
+      <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="100" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="8" t="s">
+      <c r="B32" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="8" t="s">
+      <c r="B33" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="C35" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="8" t="s">
+      <c r="B37" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="8"/>
+      <c r="C41" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="D41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="8" t="s">
+      <c r="B42" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" ht="50" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="8" t="s">
+      <c r="B43" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="C43" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="8" t="s">
+      <c r="B44" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="C44" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="8" t="s">
+      <c r="B45" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="C45" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="8" t="s">
+      <c r="B46" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="8" t="s">
+      <c r="D46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="C47" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="D47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="B40:B41"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>